<commit_message>
Resolve merge conflicts and remove deleted files
</commit_message>
<xml_diff>
--- a/docs/input_template (full for testing).xlsx
+++ b/docs/input_template (full for testing).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/slopetools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/cursor_projects/slopetools/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FECBE56-68B1-B74A-BCFC-15B8C45F923D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644E3F4F-7710-F34B-B55A-1C5FDBB558A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="780" windowWidth="32160" windowHeight="24340" activeTab="1" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
+    <workbookView xWindow="1100" yWindow="780" windowWidth="32160" windowHeight="24340" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="99">
   <si>
     <t>PySStab Input Template</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>Yo</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Does not move</t>
   </si>
 </sst>
 </file>
@@ -658,6 +664,18 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -677,18 +695,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1032,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02E090B-D957-7046-AD33-44E170F709C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,10 +1067,10 @@
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -1073,10 +1079,10 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -1085,10 +1091,10 @@
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -1097,10 +1103,10 @@
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -1109,10 +1115,10 @@
       <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
@@ -1121,10 +1127,10 @@
       <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -1133,10 +1139,10 @@
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
@@ -1145,10 +1151,10 @@
       <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
@@ -1157,11 +1163,11 @@
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="15" t="s">
@@ -1216,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4436F470-A09D-8C49-9B48-FB04FA2826AC}">
   <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -1234,26 +1240,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="25"/>
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="G2" s="21" t="s">
+      <c r="E2" s="25"/>
+      <c r="G2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="H2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="M2" s="21" t="s">
+      <c r="K2" s="25"/>
+      <c r="M2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="21"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1528,26 +1534,26 @@
       <c r="N18" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="D20" s="21" t="s">
+      <c r="B20" s="25"/>
+      <c r="D20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="G20" s="21" t="s">
+      <c r="E20" s="25"/>
+      <c r="G20" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="J20" s="21" t="s">
+      <c r="H20" s="25"/>
+      <c r="J20" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="21"/>
-      <c r="M20" s="21" t="s">
+      <c r="K20" s="25"/>
+      <c r="M20" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="N20" s="21"/>
+      <c r="N20" s="25"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1588,28 +1594,28 @@
       <c r="B22" s="3">
         <v>0</v>
       </c>
-      <c r="D22" s="25">
-        <v>0</v>
-      </c>
-      <c r="E22" s="26">
-        <v>0</v>
-      </c>
-      <c r="G22" s="25">
-        <v>0</v>
-      </c>
-      <c r="H22" s="26">
-        <v>0</v>
-      </c>
-      <c r="J22" s="25">
-        <v>0</v>
-      </c>
-      <c r="K22" s="26">
-        <v>0</v>
-      </c>
-      <c r="M22" s="25">
-        <v>0</v>
-      </c>
-      <c r="N22" s="26">
+      <c r="D22" s="18">
+        <v>0</v>
+      </c>
+      <c r="E22" s="19">
+        <v>0</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18">
+        <v>0</v>
+      </c>
+      <c r="N22" s="19">
         <v>0</v>
       </c>
     </row>
@@ -1620,28 +1626,28 @@
       <c r="B23" s="3">
         <v>0</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="20">
         <v>70</v>
       </c>
-      <c r="E23" s="28">
-        <v>0</v>
-      </c>
-      <c r="G23" s="27">
+      <c r="E23" s="21">
+        <v>0</v>
+      </c>
+      <c r="G23" s="20">
         <v>80</v>
       </c>
-      <c r="H23" s="28">
-        <v>0</v>
-      </c>
-      <c r="J23" s="27">
+      <c r="H23" s="21">
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
         <v>90</v>
       </c>
-      <c r="K23" s="28">
-        <v>0</v>
-      </c>
-      <c r="M23" s="27">
+      <c r="K23" s="21">
+        <v>0</v>
+      </c>
+      <c r="M23" s="20">
         <v>100</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1652,28 +1658,28 @@
       <c r="B24" s="3">
         <v>60</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="20">
         <v>70</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="21">
         <v>70</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="20">
         <v>80</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="21">
         <v>80</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="20">
         <v>90</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="21">
         <v>90</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="20">
         <v>100</v>
       </c>
-      <c r="N24" s="28">
+      <c r="N24" s="21">
         <v>100</v>
       </c>
     </row>
@@ -1684,28 +1690,28 @@
       <c r="B25" s="3">
         <v>100</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="20">
         <v>70</v>
       </c>
-      <c r="E25" s="28">
+      <c r="E25" s="21">
         <v>100</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="20">
         <v>80</v>
       </c>
-      <c r="H25" s="28">
+      <c r="H25" s="21">
         <v>100</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="20">
         <v>90</v>
       </c>
-      <c r="K25" s="28">
+      <c r="K25" s="21">
         <v>100</v>
       </c>
-      <c r="M25" s="27">
+      <c r="M25" s="20">
         <v>100</v>
       </c>
-      <c r="N25" s="28">
+      <c r="N25" s="21">
         <v>100</v>
       </c>
     </row>
@@ -1843,16 +1849,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1873,16 +1879,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="F2" s="22" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="J2" t="s">
         <v>91</v>
       </c>
@@ -2101,10 +2107,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="27"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2412,7 +2418,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2483,6 +2489,12 @@
       <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
@@ -2553,7 +2565,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C17" xr:uid="{AA25ABA8-BD81-3340-AC36-04678AD547F3}">
-      <formula1>$E$3:$E$4</formula1>
+      <formula1>$E$3:$E$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2581,26 +2593,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="F2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="J2" s="24" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="J2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="N2" s="24" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="N2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -2877,26 +2889,26 @@
       <c r="P13" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="F15" s="24" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="F15" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="J15" s="24" t="s">
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="J15" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="N15" s="24" t="s">
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="N15" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -3209,30 +3221,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="G2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="L2" s="24" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="L2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="Q2" s="24" t="s">
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="Q2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -3599,30 +3611,30 @@
       <c r="T13" s="3"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="G15" s="24" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="G15" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="L15" s="24" t="s">
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="L15" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="Q15" s="24" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="Q15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -3711,16 +3723,16 @@
       <c r="O17" s="3">
         <v>0</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="18">
         <v>80</v>
       </c>
-      <c r="R17" s="26">
+      <c r="R17" s="19">
         <v>80</v>
       </c>
-      <c r="S17" s="26">
-        <v>0</v>
-      </c>
-      <c r="T17" s="26">
+      <c r="S17" s="19">
+        <v>0</v>
+      </c>
+      <c r="T17" s="19">
         <v>0</v>
       </c>
     </row>
@@ -3761,16 +3773,16 @@
       <c r="O18" s="3">
         <v>0</v>
       </c>
-      <c r="Q18" s="27">
+      <c r="Q18" s="20">
         <v>29</v>
       </c>
-      <c r="R18" s="28">
+      <c r="R18" s="21">
         <v>20</v>
       </c>
-      <c r="S18" s="28">
+      <c r="S18" s="21">
         <v>800</v>
       </c>
-      <c r="T18" s="28">
+      <c r="T18" s="21">
         <v>0</v>
       </c>
     </row>
@@ -3811,16 +3823,16 @@
       <c r="O19" s="3">
         <v>0</v>
       </c>
-      <c r="Q19" s="27">
+      <c r="Q19" s="20">
         <v>41</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R19" s="21">
         <v>20</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S19" s="21">
         <v>800</v>
       </c>
-      <c r="T19" s="28">
+      <c r="T19" s="21">
         <v>0</v>
       </c>
     </row>
@@ -3861,16 +3873,16 @@
       <c r="O20" s="3">
         <v>0</v>
       </c>
-      <c r="Q20" s="27">
+      <c r="Q20" s="20">
         <v>45</v>
       </c>
-      <c r="R20" s="28">
+      <c r="R20" s="21">
         <v>20</v>
       </c>
-      <c r="S20" s="28">
-        <v>0</v>
-      </c>
-      <c r="T20" s="28">
+      <c r="S20" s="21">
+        <v>0</v>
+      </c>
+      <c r="T20" s="21">
         <v>0</v>
       </c>
     </row>
@@ -3983,30 +3995,30 @@
       <c r="T26" s="3"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="G28" s="24" t="s">
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="G28" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="L28" s="24" t="s">
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="L28" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="Q28" s="24" t="s">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="Q28" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="28"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -4059,202 +4071,202 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="25">
+      <c r="B30" s="18">
         <v>90</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="19">
         <v>90</v>
       </c>
-      <c r="D30" s="26">
-        <v>0</v>
-      </c>
-      <c r="E30" s="26">
-        <v>0</v>
-      </c>
-      <c r="G30" s="25">
+      <c r="D30" s="19">
+        <v>0</v>
+      </c>
+      <c r="E30" s="19">
+        <v>0</v>
+      </c>
+      <c r="G30" s="18">
         <v>100</v>
       </c>
-      <c r="H30" s="26">
+      <c r="H30" s="19">
         <v>100</v>
       </c>
-      <c r="I30" s="26">
-        <v>0</v>
-      </c>
-      <c r="J30" s="26">
-        <v>0</v>
-      </c>
-      <c r="L30" s="25">
+      <c r="I30" s="19">
+        <v>0</v>
+      </c>
+      <c r="J30" s="19">
+        <v>0</v>
+      </c>
+      <c r="L30" s="18">
         <v>110</v>
       </c>
-      <c r="M30" s="26">
+      <c r="M30" s="19">
         <v>110</v>
       </c>
-      <c r="N30" s="26">
-        <v>0</v>
-      </c>
-      <c r="O30" s="26">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="25">
+      <c r="N30" s="19">
+        <v>0</v>
+      </c>
+      <c r="O30" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="18">
         <v>120</v>
       </c>
-      <c r="R30" s="26">
+      <c r="R30" s="19">
         <v>120</v>
       </c>
-      <c r="S30" s="26">
-        <v>0</v>
-      </c>
-      <c r="T30" s="26">
+      <c r="S30" s="19">
+        <v>0</v>
+      </c>
+      <c r="T30" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B31" s="27">
+      <c r="B31" s="20">
         <v>29</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="21">
         <v>20</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="21">
         <v>800</v>
       </c>
-      <c r="E31" s="28">
-        <v>0</v>
-      </c>
-      <c r="G31" s="27">
+      <c r="E31" s="21">
+        <v>0</v>
+      </c>
+      <c r="G31" s="20">
         <v>29</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="21">
         <v>20</v>
       </c>
-      <c r="I31" s="28">
+      <c r="I31" s="21">
         <v>800</v>
       </c>
-      <c r="J31" s="28">
-        <v>0</v>
-      </c>
-      <c r="L31" s="27">
+      <c r="J31" s="21">
+        <v>0</v>
+      </c>
+      <c r="L31" s="20">
         <v>29</v>
       </c>
-      <c r="M31" s="28">
+      <c r="M31" s="21">
         <v>20</v>
       </c>
-      <c r="N31" s="28">
+      <c r="N31" s="21">
         <v>800</v>
       </c>
-      <c r="O31" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="27">
+      <c r="O31" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="20">
         <v>29</v>
       </c>
-      <c r="R31" s="28">
+      <c r="R31" s="21">
         <v>20</v>
       </c>
-      <c r="S31" s="28">
+      <c r="S31" s="21">
         <v>800</v>
       </c>
-      <c r="T31" s="28">
+      <c r="T31" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B32" s="27">
+      <c r="B32" s="20">
         <v>41</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="21">
         <v>20</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="21">
         <v>800</v>
       </c>
-      <c r="E32" s="28">
-        <v>0</v>
-      </c>
-      <c r="G32" s="27">
+      <c r="E32" s="21">
+        <v>0</v>
+      </c>
+      <c r="G32" s="20">
         <v>41</v>
       </c>
-      <c r="H32" s="28">
+      <c r="H32" s="21">
         <v>20</v>
       </c>
-      <c r="I32" s="28">
+      <c r="I32" s="21">
         <v>800</v>
       </c>
-      <c r="J32" s="28">
-        <v>0</v>
-      </c>
-      <c r="L32" s="27">
+      <c r="J32" s="21">
+        <v>0</v>
+      </c>
+      <c r="L32" s="20">
         <v>41</v>
       </c>
-      <c r="M32" s="28">
+      <c r="M32" s="21">
         <v>20</v>
       </c>
-      <c r="N32" s="28">
+      <c r="N32" s="21">
         <v>800</v>
       </c>
-      <c r="O32" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="27">
+      <c r="O32" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="20">
         <v>41</v>
       </c>
-      <c r="R32" s="28">
+      <c r="R32" s="21">
         <v>20</v>
       </c>
-      <c r="S32" s="28">
+      <c r="S32" s="21">
         <v>800</v>
       </c>
-      <c r="T32" s="28">
+      <c r="T32" s="21">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B33" s="27">
+      <c r="B33" s="20">
         <v>45</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="21">
         <v>20</v>
       </c>
-      <c r="D33" s="28">
-        <v>0</v>
-      </c>
-      <c r="E33" s="28">
-        <v>0</v>
-      </c>
-      <c r="G33" s="27">
+      <c r="D33" s="21">
+        <v>0</v>
+      </c>
+      <c r="E33" s="21">
+        <v>0</v>
+      </c>
+      <c r="G33" s="20">
         <v>45</v>
       </c>
-      <c r="H33" s="28">
+      <c r="H33" s="21">
         <v>20</v>
       </c>
-      <c r="I33" s="28">
-        <v>0</v>
-      </c>
-      <c r="J33" s="28">
-        <v>0</v>
-      </c>
-      <c r="L33" s="27">
+      <c r="I33" s="21">
+        <v>0</v>
+      </c>
+      <c r="J33" s="21">
+        <v>0</v>
+      </c>
+      <c r="L33" s="20">
         <v>45</v>
       </c>
-      <c r="M33" s="28">
+      <c r="M33" s="21">
         <v>20</v>
       </c>
-      <c r="N33" s="28">
-        <v>0</v>
-      </c>
-      <c r="O33" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="27">
+      <c r="N33" s="21">
+        <v>0</v>
+      </c>
+      <c r="O33" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="20">
         <v>45</v>
       </c>
-      <c r="R33" s="28">
+      <c r="R33" s="21">
         <v>20</v>
       </c>
-      <c r="S33" s="28">
-        <v>0</v>
-      </c>
-      <c r="T33" s="28">
+      <c r="S33" s="21">
+        <v>0</v>
+      </c>
+      <c r="T33" s="21">
         <v>0</v>
       </c>
     </row>

</xml_diff>